<commit_message>
Update information model for new SSP
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -1,21 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="14550" windowHeight="7290"/>
+    <workbookView xWindow="6360" yWindow="3340" windowWidth="24620" windowHeight="13040"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
     <sheet name="Court Case Filing Update" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jim Douglas</author>
+  </authors>
+  <commentList>
+    <comment ref="C29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jim Douglas:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="243">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -414,9 +453,6 @@
   </si>
   <si>
     <t>/ccu-filing-doc:CourtCaseFilingDocument/j:JudicialOfficial/j:JudicialOfficialCategoryText</t>
-  </si>
-  <si>
-    <t>REMOVE</t>
   </si>
   <si>
     <t>Charge Domestic Violence indicator</t>
@@ -753,7 +789,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -873,27 +909,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
       <sz val="9"/>
+      <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <strike/>
+      <b/>
       <sz val="9"/>
-      <color rgb="FFFF0000"/>
+      <color indexed="81"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="9"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1019,7 +1045,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1067,15 +1093,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1406,23 +1423,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="16.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="1" customWidth="1"/>
     <col min="5" max="5" width="157" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="6" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="16">
         <v>42255</v>
       </c>
@@ -1436,716 +1453,713 @@
         <v>9</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
+    <row r="3" spans="1:5">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
       <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
       <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="20"/>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="14" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20"/>
+    <row r="10" spans="1:5">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="10" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="20"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="20"/>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="10" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C16" s="12" t="s">
         <v>0</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20" t="s">
-        <v>135</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17" t="s">
+        <v>134</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="B18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="14" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C20" s="12" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="5"/>
       <c r="E20" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="A21" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="A22" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="A23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="A24" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C25" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C26" s="12" t="s">
         <v>26</v>
       </c>
       <c r="D26" s="5"/>
       <c r="E26" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C27" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="26.25" customHeight="1">
       <c r="C28" s="12" t="s">
         <v>29</v>
       </c>
       <c r="D28" s="5"/>
       <c r="E28" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="12">
+      <c r="C29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="18"/>
-      <c r="E29" s="19" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C30" s="12" t="s">
         <v>31</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C31" s="12" t="s">
         <v>64</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C32" s="12" t="s">
         <v>61</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C33" s="12" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C34" s="12" t="s">
         <v>63</v>
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C35" s="12" t="s">
         <v>65</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1">
       <c r="C36" s="12" t="s">
         <v>66</v>
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C37" s="12" t="s">
         <v>67</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C38" s="12" t="s">
         <v>68</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="20"/>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
       <c r="C39" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C40" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C41" s="12" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C42" s="12" t="s">
         <v>16</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C43" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="6"/>
       <c r="E43" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C44" s="12" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C45" s="12" t="s">
         <v>22</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C46" s="12" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C47" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D47" s="6"/>
       <c r="E47" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C48" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D48" s="6"/>
       <c r="E48" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C49" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="B50" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D50" s="6"/>
       <c r="E50" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="A51" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D51" s="6"/>
       <c r="E51" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="17"/>
+      <c r="B52" s="17"/>
       <c r="C52" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D52" s="7"/>
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C53" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D53" s="6"/>
       <c r="E53" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C54" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D54" s="6"/>
       <c r="E54" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C55" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D55" s="6"/>
       <c r="E55" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C56" s="12" t="s">
         <v>41</v>
       </c>
       <c r="D56" s="6"/>
       <c r="E56" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C57" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D57" s="6"/>
       <c r="E57" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C58" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C59" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C60" s="12" t="s">
         <v>45</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C61" s="12" t="s">
         <v>48</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C62" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C63" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="2" customFormat="1" ht="12">
       <c r="C64" s="12" t="s">
         <v>49</v>
       </c>
       <c r="D64" s="6"/>
       <c r="E64" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" s="2" customFormat="1" ht="12">
       <c r="C65" s="12" t="s">
         <v>50</v>
       </c>
       <c r="D65" s="6"/>
       <c r="E65" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" s="2" customFormat="1" ht="12">
       <c r="C66" s="12" t="s">
         <v>51</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="2" customFormat="1" ht="12">
       <c r="A67" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="2" customFormat="1" ht="12">
       <c r="A68" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D68" s="6"/>
       <c r="E68" s="6" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="2" customFormat="1" ht="12">
       <c r="A69" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D69" s="6"/>
       <c r="E69" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="17"/>
+      <c r="B70" s="17"/>
       <c r="C70" s="14" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="7"/>
       <c r="E70" s="9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="17"/>
+      <c r="B71" s="17"/>
       <c r="C71" s="10" t="s">
         <v>69</v>
       </c>
       <c r="D71" s="15"/>
       <c r="E71" s="3" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="17"/>
+      <c r="B72" s="17"/>
       <c r="C72" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D72" s="15"/>
       <c r="E72" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="12" t="s">
@@ -2153,7 +2167,7 @@
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -2162,7 +2176,7 @@
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="12" t="s">
@@ -2170,7 +2184,7 @@
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
@@ -2179,7 +2193,7 @@
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="12" t="s">
@@ -2187,7 +2201,7 @@
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
@@ -2196,7 +2210,7 @@
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="12" t="s">
@@ -2204,7 +2218,7 @@
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -2213,7 +2227,7 @@
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="14" t="s">
@@ -2221,7 +2235,7 @@
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -2230,7 +2244,7 @@
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="10" t="s">
@@ -2238,7 +2252,7 @@
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
@@ -2247,7 +2261,7 @@
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="10" t="s">
@@ -2255,7 +2269,7 @@
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -2264,7 +2278,7 @@
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="10" t="s">
@@ -2272,7 +2286,7 @@
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
@@ -2281,7 +2295,7 @@
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="10" t="s">
@@ -2289,7 +2303,7 @@
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -2298,15 +2312,15 @@
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D82" s="9"/>
       <c r="E82" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -2315,15 +2329,15 @@
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -2332,17 +2346,17 @@
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11">
       <c r="A84" s="3"/>
       <c r="B84" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -2351,17 +2365,17 @@
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11">
       <c r="A85" s="3"/>
       <c r="B85" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C85" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -2370,17 +2384,17 @@
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11">
       <c r="A86" s="3"/>
       <c r="B86" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C86" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -2389,17 +2403,17 @@
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11">
       <c r="A87" s="3"/>
       <c r="B87" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -2408,17 +2422,17 @@
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11">
       <c r="A88" s="3"/>
       <c r="B88" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C88" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -2427,17 +2441,17 @@
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11">
       <c r="A89" s="3"/>
       <c r="B89" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C89" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -2446,17 +2460,17 @@
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11">
       <c r="A90" s="3"/>
       <c r="B90" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D90" s="9"/>
       <c r="E90" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -2465,17 +2479,17 @@
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11">
       <c r="A91" s="3"/>
       <c r="B91" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -2484,17 +2498,17 @@
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11">
       <c r="A92" s="3"/>
       <c r="B92" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C92" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -2503,17 +2517,17 @@
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11">
       <c r="A93" s="3"/>
       <c r="B93" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D93" s="9"/>
       <c r="E93" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -2522,17 +2536,17 @@
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11">
       <c r="A94" s="3"/>
       <c r="B94" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -2541,17 +2555,17 @@
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11">
       <c r="A95" s="3"/>
       <c r="B95" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -2560,17 +2574,17 @@
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11">
       <c r="A96" s="3"/>
       <c r="B96" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D96" s="9"/>
       <c r="E96" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -2579,17 +2593,17 @@
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11">
       <c r="A97" s="3"/>
       <c r="B97" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
@@ -2598,7 +2612,7 @@
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="10"/>
@@ -2611,7 +2625,7 @@
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="10"/>
@@ -2624,7 +2638,7 @@
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="10"/>
@@ -2637,7 +2651,7 @@
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="10"/>
@@ -2650,7 +2664,7 @@
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="10"/>
@@ -2663,7 +2677,7 @@
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="10"/>
@@ -2676,7 +2690,7 @@
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="10"/>
@@ -2689,7 +2703,7 @@
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="10"/>
@@ -2702,7 +2716,7 @@
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="10"/>
@@ -2715,7 +2729,7 @@
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="10"/>
@@ -2730,7 +2744,13 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2742,15 +2762,15 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="152.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="32.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="152.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
@@ -2761,14 +2781,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="12" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -2777,7 +2797,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="12" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -2786,7 +2806,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="12" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -2795,7 +2815,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="12" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -2804,7 +2824,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="12" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -2813,14 +2833,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="12" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
@@ -2829,7 +2849,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="12" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
@@ -2838,7 +2858,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="12" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -2847,7 +2867,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="12" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
@@ -2856,7 +2876,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="12" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
@@ -2865,7 +2885,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="12" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
@@ -2874,7 +2894,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="12" t="s">
         <v>0</v>
       </c>
@@ -2883,14 +2903,14 @@
         <v>82</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A17" s="12" t="s">
         <v>3</v>
       </c>
@@ -2899,7 +2919,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
@@ -2908,7 +2928,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
@@ -2917,7 +2937,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A20" s="12" t="s">
         <v>28</v>
       </c>
@@ -2926,7 +2946,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A21" s="12" t="s">
         <v>29</v>
       </c>
@@ -2935,7 +2955,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A22" s="12" t="s">
         <v>30</v>
       </c>
@@ -2944,7 +2964,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
@@ -2953,7 +2973,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A24" s="12" t="s">
         <v>64</v>
       </c>
@@ -2962,7 +2982,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A25" s="12" t="s">
         <v>61</v>
       </c>
@@ -2971,7 +2991,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A26" s="12" t="s">
         <v>62</v>
       </c>
@@ -2980,7 +3000,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A27" s="12" t="s">
         <v>63</v>
       </c>
@@ -2989,7 +3009,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A28" s="12" t="s">
         <v>65</v>
       </c>
@@ -2998,7 +3018,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A29" s="12" t="s">
         <v>66</v>
       </c>
@@ -3007,7 +3027,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A30" s="12" t="s">
         <v>67</v>
       </c>
@@ -3016,7 +3036,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A31" s="12" t="s">
         <v>68</v>
       </c>
@@ -3025,14 +3045,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
@@ -3041,7 +3061,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A34" s="12" t="s">
         <v>15</v>
       </c>
@@ -3050,7 +3070,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
@@ -3059,7 +3079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A36" s="12" t="s">
         <v>17</v>
       </c>
@@ -3068,7 +3088,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A37" s="12" t="s">
         <v>18</v>
       </c>
@@ -3077,7 +3097,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A38" s="12" t="s">
         <v>22</v>
       </c>
@@ -3086,7 +3106,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A39" s="12" t="s">
         <v>19</v>
       </c>
@@ -3095,7 +3115,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A40" s="12" t="s">
         <v>23</v>
       </c>
@@ -3104,7 +3124,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A41" s="12" t="s">
         <v>24</v>
       </c>
@@ -3113,7 +3133,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A42" s="12" t="s">
         <v>25</v>
       </c>
@@ -3122,14 +3142,14 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3">
       <c r="A43" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="9"/>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A44" s="12" t="s">
         <v>38</v>
       </c>
@@ -3138,7 +3158,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A45" s="12" t="s">
         <v>39</v>
       </c>
@@ -3147,7 +3167,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A46" s="12" t="s">
         <v>40</v>
       </c>
@@ -3156,7 +3176,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A47" s="12" t="s">
         <v>41</v>
       </c>
@@ -3165,7 +3185,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A48" s="12" t="s">
         <v>42</v>
       </c>
@@ -3174,7 +3194,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A49" s="12" t="s">
         <v>43</v>
       </c>
@@ -3183,7 +3203,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A50" s="5" t="s">
         <v>44</v>
       </c>
@@ -3192,7 +3212,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A51" s="12" t="s">
         <v>45</v>
       </c>
@@ -3201,7 +3221,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A52" s="12" t="s">
         <v>48</v>
       </c>
@@ -3210,7 +3230,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A53" s="12" t="s">
         <v>46</v>
       </c>
@@ -3219,7 +3239,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A54" s="12" t="s">
         <v>47</v>
       </c>
@@ -3228,7 +3248,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
@@ -3237,7 +3257,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A56" s="12" t="s">
         <v>50</v>
       </c>
@@ -3246,7 +3266,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" s="2" customFormat="1" ht="12">
       <c r="A57" s="5" t="s">
         <v>51</v>
       </c>
@@ -3255,7 +3275,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" s="14" t="s">
         <v>7</v>
       </c>
@@ -3264,7 +3284,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="12" customHeight="1">
       <c r="A59" s="10" t="s">
         <v>69</v>
       </c>
@@ -3273,7 +3293,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="12" customHeight="1">
       <c r="A60" s="12" t="s">
         <v>52</v>
       </c>
@@ -3282,7 +3302,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="12" customHeight="1">
       <c r="A61" s="12" t="s">
         <v>53</v>
       </c>
@@ -3291,7 +3311,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="12" customHeight="1">
       <c r="A62" s="12" t="s">
         <v>54</v>
       </c>
@@ -3300,7 +3320,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="12" customHeight="1">
       <c r="A63" s="12" t="s">
         <v>55</v>
       </c>
@@ -3309,7 +3329,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="12" customHeight="1">
       <c r="A64" s="12" t="s">
         <v>56</v>
       </c>
@@ -3318,7 +3338,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="14" t="s">
         <v>8</v>
       </c>
@@ -3327,7 +3347,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="12" customHeight="1">
       <c r="A66" s="10" t="s">
         <v>57</v>
       </c>
@@ -3335,7 +3355,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="12" customHeight="1">
       <c r="A67" s="10" t="s">
         <v>58</v>
       </c>
@@ -3343,7 +3363,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="12" customHeight="1">
       <c r="A68" s="10" t="s">
         <v>59</v>
       </c>
@@ -3351,7 +3371,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="12" customHeight="1">
       <c r="A69" s="10" t="s">
         <v>60</v>
       </c>
@@ -3359,54 +3379,59 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" s="10"/>
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="10"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" s="10"/>
       <c r="C72" s="3"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="10"/>
       <c r="C73" s="3"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="10"/>
       <c r="C74" s="3"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3">
       <c r="C75" s="3"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="C76" s="3"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3">
       <c r="C78" s="3"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3">
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="C80" s="3"/>
     </row>
-    <row r="81" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" s="1" customFormat="1">
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" s="1" customFormat="1">
       <c r="C82" s="3"/>
     </row>
-    <row r="83" spans="3:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" s="1" customFormat="1">
       <c r="C83" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added alaska and hawaii "impl" folder.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Case_Filing_Decision_Reporting/artifacts/service_model/information_model/IEPD/documentation/Mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="3340" windowWidth="24620" windowHeight="13040"/>
+    <workbookView xWindow="9840" yWindow="2320" windowWidth="24620" windowHeight="13040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>Jim Douglas</author>
   </authors>
   <commentList>
-    <comment ref="C29" authorId="0">
+    <comment ref="A29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="242">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -456,9 +456,6 @@
   </si>
   <si>
     <t>Charge Domestic Violence indicator</t>
-  </si>
-  <si>
-    <t>ADD</t>
   </si>
   <si>
     <t>Digitized Signature ?</t>
@@ -1045,7 +1042,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1090,12 +1087,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1424,1323 +1415,1142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K107"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="16.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" style="1" customWidth="1"/>
-    <col min="5" max="5" width="157" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="29.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="1" customWidth="1"/>
+    <col min="3" max="3" width="157" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="16">
-        <v>42255</v>
-      </c>
-      <c r="B1" s="16">
-        <v>42269</v>
-      </c>
-      <c r="C1" s="11" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="14" t="s">
+      <c r="C1" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="10" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="3" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="17" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A16" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A18" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A20" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A21" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A22" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A23" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A24" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A25" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A26" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A27" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="2" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A28" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A30" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A31" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A32" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A33" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A34" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A35" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="2" customFormat="1" ht="22.5" customHeight="1">
+      <c r="A36" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A37" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A38" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A40" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A41" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A42" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A43" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A45" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A46" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A47" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A48" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A49" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A50" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A51" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A53" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A54" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A55" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A56" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A57" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A58" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A59" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="10" t="s">
+      <c r="B59" s="6"/>
+      <c r="C59" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A60" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A61" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A62" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A63" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" s="2" customFormat="1" ht="12">
+      <c r="A64" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="2" customFormat="1" ht="12">
+      <c r="A65" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="6" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="2" customFormat="1" ht="12">
+      <c r="A66" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="2" customFormat="1" ht="12">
+      <c r="A67" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="2" customFormat="1" ht="12">
+      <c r="A68" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="2" customFormat="1" ht="12">
+      <c r="A69" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="B18" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="A21" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="A22" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="A23" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="A24" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C25" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C26" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C27" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="26.25" customHeight="1">
-      <c r="C28" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C29" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="6" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C30" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C31" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D31" s="5"/>
-      <c r="E31" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C32" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C33" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C34" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="5"/>
-      <c r="E34" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C35" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="22.5" customHeight="1">
-      <c r="C36" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C37" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C38" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="17"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C40" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C41" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C42" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C43" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C44" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C45" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C46" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C47" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C48" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C49" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="B50" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6" t="s">
+      <c r="B69" s="6"/>
+      <c r="C69" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="7"/>
+      <c r="C70" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71" s="15"/>
+      <c r="C71" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B72" s="15"/>
+      <c r="C72" s="3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="A51" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="7"/>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C53" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6" t="s">
+    <row r="73" spans="1:9">
+      <c r="A73" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C54" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C55" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C56" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C57" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C58" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C59" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C60" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C61" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C62" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C63" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="2" customFormat="1" ht="12">
-      <c r="C64" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="2" customFormat="1" ht="12">
-      <c r="C65" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" s="2" customFormat="1" ht="12">
-      <c r="C66" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="2" customFormat="1" ht="12">
-      <c r="A67" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" s="2" customFormat="1" ht="12">
-      <c r="A68" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" s="2" customFormat="1" ht="12">
-      <c r="A69" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="A70" s="17"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11">
-      <c r="A71" s="17"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" s="15"/>
-      <c r="E71" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11">
-      <c r="A72" s="17"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D72" s="15"/>
-      <c r="E72" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11">
-      <c r="A73" s="3"/>
-      <c r="B73" s="3"/>
-      <c r="C73" s="12" t="s">
-        <v>53</v>
-      </c>
       <c r="D73" s="3"/>
-      <c r="E73" s="3" t="s">
-        <v>202</v>
-      </c>
+      <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
       <c r="I73" s="3"/>
-      <c r="J73" s="3"/>
-      <c r="K73" s="3"/>
-    </row>
-    <row r="74" spans="1:11">
-      <c r="A74" s="3"/>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="12" t="s">
+        <v>54</v>
+      </c>
       <c r="B74" s="3"/>
-      <c r="C74" s="12" t="s">
-        <v>54</v>
+      <c r="C74" s="3" t="s">
+        <v>202</v>
       </c>
       <c r="D74" s="3"/>
-      <c r="E74" s="3" t="s">
-        <v>203</v>
-      </c>
+      <c r="E74" s="3"/>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
-      <c r="J74" s="3"/>
-      <c r="K74" s="3"/>
-    </row>
-    <row r="75" spans="1:11">
-      <c r="A75" s="3"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="12" t="s">
+        <v>55</v>
+      </c>
       <c r="B75" s="3"/>
-      <c r="C75" s="12" t="s">
-        <v>55</v>
+      <c r="C75" s="3" t="s">
+        <v>203</v>
       </c>
       <c r="D75" s="3"/>
-      <c r="E75" s="3" t="s">
-        <v>204</v>
-      </c>
+      <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
       <c r="I75" s="3"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="3"/>
-    </row>
-    <row r="76" spans="1:11">
-      <c r="A76" s="3"/>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="B76" s="3"/>
-      <c r="C76" s="12" t="s">
-        <v>56</v>
+      <c r="C76" s="3" t="s">
+        <v>204</v>
       </c>
       <c r="D76" s="3"/>
-      <c r="E76" s="3" t="s">
-        <v>205</v>
-      </c>
+      <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
-    </row>
-    <row r="77" spans="1:11">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="14" t="s">
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9" t="s">
-        <v>217</v>
-      </c>
+      <c r="B77" s="9"/>
+      <c r="C77" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-    </row>
-    <row r="78" spans="1:11">
-      <c r="A78" s="3"/>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="10" t="s">
+        <v>57</v>
+      </c>
       <c r="B78" s="3"/>
-      <c r="C78" s="10" t="s">
-        <v>57</v>
+      <c r="C78" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="D78" s="3"/>
-      <c r="E78" s="3" t="s">
-        <v>218</v>
-      </c>
+      <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
       <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-    </row>
-    <row r="79" spans="1:11">
-      <c r="A79" s="3"/>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="B79" s="3"/>
-      <c r="C79" s="10" t="s">
-        <v>58</v>
+      <c r="C79" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="D79" s="3"/>
-      <c r="E79" s="3" t="s">
-        <v>219</v>
-      </c>
+      <c r="E79" s="3"/>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-    </row>
-    <row r="80" spans="1:11">
-      <c r="A80" s="3"/>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="10" t="s">
+        <v>59</v>
+      </c>
       <c r="B80" s="3"/>
-      <c r="C80" s="10" t="s">
-        <v>59</v>
+      <c r="C80" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="D80" s="3"/>
-      <c r="E80" s="3" t="s">
-        <v>220</v>
-      </c>
+      <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
-      <c r="J80" s="3"/>
-      <c r="K80" s="3"/>
-    </row>
-    <row r="81" spans="1:11">
-      <c r="A81" s="3"/>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="10" t="s">
+        <v>60</v>
+      </c>
       <c r="B81" s="3"/>
-      <c r="C81" s="10" t="s">
-        <v>60</v>
+      <c r="C81" s="3" t="s">
+        <v>220</v>
       </c>
       <c r="D81" s="3"/>
-      <c r="E81" s="3" t="s">
-        <v>221</v>
-      </c>
+      <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
-      <c r="J81" s="3"/>
-      <c r="K81" s="3"/>
-    </row>
-    <row r="82" spans="1:11">
-      <c r="A82" s="3"/>
-      <c r="B82" s="3"/>
-      <c r="C82" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9" t="s">
-        <v>222</v>
-      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-    </row>
-    <row r="83" spans="1:11">
-      <c r="A83" s="3"/>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="10" t="s">
+        <v>145</v>
+      </c>
       <c r="B83" s="3"/>
-      <c r="C83" s="10" t="s">
-        <v>146</v>
+      <c r="C83" s="3" t="s">
+        <v>222</v>
       </c>
       <c r="D83" s="3"/>
-      <c r="E83" s="3" t="s">
-        <v>223</v>
-      </c>
+      <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
-      <c r="K83" s="3"/>
-    </row>
-    <row r="84" spans="1:11">
-      <c r="A84" s="3"/>
-      <c r="B84" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D84" s="9"/>
-      <c r="E84" s="9" t="s">
-        <v>224</v>
-      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
-      <c r="K84" s="3"/>
-    </row>
-    <row r="85" spans="1:11">
-      <c r="A85" s="3"/>
-      <c r="B85" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>148</v>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B85" s="3"/>
+      <c r="C85" s="3" t="s">
+        <v>224</v>
       </c>
       <c r="D85" s="3"/>
-      <c r="E85" s="3" t="s">
-        <v>225</v>
-      </c>
+      <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
-    </row>
-    <row r="86" spans="1:11">
-      <c r="A86" s="3"/>
-      <c r="B86" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>149</v>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B86" s="3"/>
+      <c r="C86" s="3" t="s">
+        <v>225</v>
       </c>
       <c r="D86" s="3"/>
-      <c r="E86" s="3" t="s">
-        <v>226</v>
-      </c>
+      <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
-      <c r="K86" s="3"/>
-    </row>
-    <row r="87" spans="1:11">
-      <c r="A87" s="3"/>
-      <c r="B87" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>150</v>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B87" s="3"/>
+      <c r="C87" s="3" t="s">
+        <v>226</v>
       </c>
       <c r="D87" s="3"/>
-      <c r="E87" s="3" t="s">
-        <v>227</v>
-      </c>
+      <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
-      <c r="J87" s="3"/>
-      <c r="K87" s="3"/>
-    </row>
-    <row r="88" spans="1:11">
-      <c r="A88" s="3"/>
-      <c r="B88" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>151</v>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B88" s="3"/>
+      <c r="C88" s="3" t="s">
+        <v>227</v>
       </c>
       <c r="D88" s="3"/>
-      <c r="E88" s="3" t="s">
-        <v>228</v>
-      </c>
+      <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
-      <c r="J88" s="3"/>
-      <c r="K88" s="3"/>
-    </row>
-    <row r="89" spans="1:11">
-      <c r="A89" s="3"/>
-      <c r="B89" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>152</v>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="D89" s="3"/>
-      <c r="E89" s="3" t="s">
-        <v>229</v>
-      </c>
+      <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
-      <c r="J89" s="3"/>
-      <c r="K89" s="3"/>
-    </row>
-    <row r="90" spans="1:11">
-      <c r="A90" s="3"/>
-      <c r="B90" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9" t="s">
-        <v>230</v>
-      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
-      <c r="K90" s="3"/>
-    </row>
-    <row r="91" spans="1:11">
-      <c r="A91" s="3"/>
-      <c r="B91" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C91" s="10" t="s">
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="10" t="s">
         <v>7</v>
       </c>
+      <c r="B91" s="3"/>
+      <c r="C91" s="3" t="s">
+        <v>230</v>
+      </c>
       <c r="D91" s="3"/>
-      <c r="E91" s="3" t="s">
-        <v>231</v>
-      </c>
+      <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
-      <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
-    </row>
-    <row r="92" spans="1:11">
-      <c r="A92" s="3"/>
-      <c r="B92" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>147</v>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" s="3"/>
+      <c r="C92" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="D92" s="3"/>
-      <c r="E92" s="3" t="s">
-        <v>232</v>
-      </c>
+      <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
-      <c r="K92" s="3"/>
-    </row>
-    <row r="93" spans="1:11">
-      <c r="A93" s="3"/>
-      <c r="B93" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9" t="s">
-        <v>230</v>
-      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="B93" s="9"/>
+      <c r="C93" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
-      <c r="K93" s="3"/>
-    </row>
-    <row r="94" spans="1:11">
-      <c r="A94" s="3"/>
-      <c r="B94" s="6" t="s">
-        <v>134</v>
-      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B94" s="3"/>
       <c r="C94" s="3" t="s">
-        <v>155</v>
+        <v>232</v>
       </c>
       <c r="D94" s="3"/>
-      <c r="E94" s="3" t="s">
-        <v>233</v>
-      </c>
+      <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
-      <c r="J94" s="3"/>
-      <c r="K94" s="3"/>
-    </row>
-    <row r="95" spans="1:11">
-      <c r="A95" s="3"/>
-      <c r="B95" s="6" t="s">
-        <v>134</v>
-      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B95" s="3"/>
       <c r="C95" s="3" t="s">
-        <v>147</v>
+        <v>233</v>
       </c>
       <c r="D95" s="3"/>
-      <c r="E95" s="3" t="s">
-        <v>234</v>
-      </c>
+      <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="3"/>
-    </row>
-    <row r="96" spans="1:11">
-      <c r="A96" s="3"/>
-      <c r="B96" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D96" s="9"/>
-      <c r="E96" s="9" t="s">
-        <v>241</v>
-      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D96" s="3"/>
+      <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-    </row>
-    <row r="97" spans="1:11">
-      <c r="A97" s="3"/>
-      <c r="B97" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>158</v>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B97" s="3"/>
+      <c r="C97" s="3" t="s">
+        <v>241</v>
       </c>
       <c r="D97" s="3"/>
-      <c r="E97" s="3" t="s">
-        <v>242</v>
-      </c>
+      <c r="E97" s="3"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
-      <c r="J97" s="3"/>
-      <c r="K97" s="3"/>
-    </row>
-    <row r="98" spans="1:11">
-      <c r="A98" s="3"/>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="10"/>
       <c r="B98" s="3"/>
-      <c r="C98" s="10"/>
+      <c r="C98" s="3"/>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-    </row>
-    <row r="99" spans="1:11">
-      <c r="A99" s="3"/>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="10"/>
       <c r="B99" s="3"/>
-      <c r="C99" s="10"/>
+      <c r="C99" s="3"/>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-    </row>
-    <row r="100" spans="1:11">
-      <c r="A100" s="3"/>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="10"/>
       <c r="B100" s="3"/>
-      <c r="C100" s="10"/>
+      <c r="C100" s="3"/>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
-      <c r="K100" s="3"/>
-    </row>
-    <row r="101" spans="1:11">
-      <c r="A101" s="3"/>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="10"/>
       <c r="B101" s="3"/>
-      <c r="C101" s="10"/>
+      <c r="C101" s="3"/>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3"/>
-    </row>
-    <row r="102" spans="1:11">
-      <c r="A102" s="3"/>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" s="10"/>
       <c r="B102" s="3"/>
-      <c r="C102" s="10"/>
+      <c r="C102" s="3"/>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-    </row>
-    <row r="103" spans="1:11">
-      <c r="A103" s="3"/>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" s="10"/>
       <c r="B103" s="3"/>
-      <c r="C103" s="10"/>
+      <c r="C103" s="3"/>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
-      <c r="J103" s="3"/>
-      <c r="K103" s="3"/>
-    </row>
-    <row r="104" spans="1:11">
-      <c r="A104" s="3"/>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="10"/>
       <c r="B104" s="3"/>
-      <c r="C104" s="10"/>
+      <c r="C104" s="3"/>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
-      <c r="J104" s="3"/>
-      <c r="K104" s="3"/>
-    </row>
-    <row r="105" spans="1:11">
-      <c r="A105" s="3"/>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="10"/>
       <c r="B105" s="3"/>
-      <c r="C105" s="10"/>
+      <c r="C105" s="3"/>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="3"/>
-    </row>
-    <row r="106" spans="1:11">
-      <c r="A106" s="3"/>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="10"/>
       <c r="B106" s="3"/>
-      <c r="C106" s="10"/>
+      <c r="C106" s="3"/>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
-      <c r="J106" s="3"/>
-      <c r="K106" s="3"/>
-    </row>
-    <row r="107" spans="1:11">
-      <c r="A107" s="3"/>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="10"/>
       <c r="B107" s="3"/>
-      <c r="C107" s="10"/>
+      <c r="C107" s="3"/>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
-      <c r="J107" s="3"/>
-      <c r="K107" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2758,7 +2568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>